<commit_message>
Errors in ATTRIBUTES REMOVED
</commit_message>
<xml_diff>
--- a/Results/new/Result_class_freq_2.xlsx
+++ b/Results/new/Result_class_freq_2.xlsx
@@ -79,9 +79,6 @@
     <t>LOGISTIC REGRESSION</t>
   </si>
   <si>
-    <t>REFILL_COUNT</t>
-  </si>
-  <si>
     <t>SVM(LINEAR)</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>BUTRANS ONLY : MEDIAN = 2</t>
+  </si>
+  <si>
+    <t>CLASS DRUG</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -629,13 +629,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F6" s="1">
         <v>53.670299999999997</v>
@@ -646,13 +646,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="1">
         <v>54.6265</v>
@@ -663,13 +663,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F8" s="3">
         <v>56.629600000000003</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F9" s="1">
         <v>56.423900000000003</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>29</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>31</v>
@@ -718,22 +718,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>